<commit_message>
templates updated and so raw material
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/07-BulkUploadMachineType.xlsx
+++ b/documents/templates/bulk-upload/07-BulkUploadMachineType.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2097016-C3AC-7843-869E-314D89C8C9D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFFD8CA-3B97-E244-9E90-6BFD7352A5C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{03CB352A-59C4-E548-9F5B-8794D5B56636}"/>
   </bookViews>
@@ -33,22 +33,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Circular Saw</t>
-  </si>
-  <si>
-    <t>CNC</t>
-  </si>
-  <si>
-    <t>NC</t>
-  </si>
-  <si>
-    <t>MANUAL</t>
-  </si>
-  <si>
     <t>Machine Type</t>
   </si>
   <si>
-    <t>Band Saw</t>
+    <t>Tube cutting manual</t>
+  </si>
+  <si>
+    <t>Pedrazzoli tube cutting</t>
+  </si>
+  <si>
+    <t>Plasma</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>Horizontal tube bending</t>
   </si>
 </sst>
 </file>
@@ -403,42 +403,42 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bulk insertion is completed
</commit_message>
<xml_diff>
--- a/documents/templates/bulk-upload/07-BulkUploadMachineType.xlsx
+++ b/documents/templates/bulk-upload/07-BulkUploadMachineType.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFFD8CA-3B97-E244-9E90-6BFD7352A5C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539C6D99-7C5B-814F-8DD6-296AEDF590A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{03CB352A-59C4-E548-9F5B-8794D5B56636}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Machine Type</t>
   </si>
@@ -49,6 +49,33 @@
   </si>
   <si>
     <t>Horizontal tube bending</t>
+  </si>
+  <si>
+    <t>Vertical tube bending</t>
+  </si>
+  <si>
+    <t>Shearing</t>
+  </si>
+  <si>
+    <t>Sheet bending</t>
+  </si>
+  <si>
+    <t>Notching machine</t>
+  </si>
+  <si>
+    <t>Mechanical press machine</t>
+  </si>
+  <si>
+    <t>hydraullic press machine</t>
+  </si>
+  <si>
+    <t>Speedy seamer</t>
+  </si>
+  <si>
+    <t>Drilling machine</t>
+  </si>
+  <si>
+    <t>Vertical band saw</t>
   </si>
 </sst>
 </file>
@@ -400,15 +427,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6603046D-2B86-B141-B65D-D932A8F5B98E}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -441,6 +468,51 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>